<commit_message>
Fixed the issues raised by the PMS team, except button overlays
</commit_message>
<xml_diff>
--- a/bootstrap/init_data/ListOfAMCUsers_nav.xlsx
+++ b/bootstrap/init_data/ListOfAMCUsers_nav.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmudgil/projects/pms-aif/pmsaif-web-Jun-2024/init_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmudgil/projects/pms-aif/pmsportal_aug_2024/bootstrap/init_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228676CD-2391-A94C-9948-375B148CC7A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B958F3-1CCA-A04E-9B40-8856405B61F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14460" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29840" yWindow="-21100" windowWidth="19080" windowHeight="20940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AMC Users" sheetId="2" r:id="rId1"/>
@@ -2151,7 +2151,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2161,6 +2161,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2196,7 +2202,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2267,13 +2273,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2593,8 +2614,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E182" sqref="E182"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2622,7 +2644,7 @@
     <col min="22" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>151</v>
       </c>
@@ -2638,7 +2660,7 @@
       <c r="E1" s="4" t="s">
         <v>666</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="4" t="s">
         <v>667</v>
       </c>
       <c r="G1" s="5" t="s">
@@ -2647,65 +2669,74 @@
       <c r="H1" s="4" t="s">
         <v>669</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="4" t="s">
         <v>670</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="24" t="s">
         <v>671</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="25" t="s">
         <v>672</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="L1" s="25" t="s">
         <v>673</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="M1" s="24" t="s">
         <v>674</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="N1" s="25" t="s">
         <v>675</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="O1" s="25" t="s">
         <v>676</v>
       </c>
-      <c r="P1" s="25" t="s">
+      <c r="P1" s="24" t="s">
         <v>677</v>
       </c>
-      <c r="Q1" s="26" t="s">
+      <c r="Q1" s="25" t="s">
         <v>678</v>
       </c>
-      <c r="R1" s="26" t="s">
+      <c r="R1" s="25" t="s">
         <v>679</v>
       </c>
-      <c r="S1" s="25" t="s">
+      <c r="S1" s="24" t="s">
         <v>680</v>
       </c>
-      <c r="T1" s="26" t="s">
+      <c r="T1" s="25" t="s">
         <v>681</v>
       </c>
-      <c r="U1" s="26" t="s">
+      <c r="U1" s="25" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+    <row r="2" spans="1:21" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="26">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="26">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="27" t="s">
         <v>408</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="26" t="s">
         <v>409</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="30" t="s">
         <v>308</v>
       </c>
+      <c r="G2" s="27"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="27"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="27"/>
+      <c r="U2" s="29"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -3188,25 +3219,34 @@
         <v>662</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
+    <row r="22" spans="1:21" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="26">
         <v>21</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="26">
         <v>21</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="27" t="s">
         <v>457</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="26" t="s">
         <v>409</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="31" t="s">
         <v>326</v>
       </c>
+      <c r="G22" s="27"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="27"/>
+      <c r="M22" s="27"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="27"/>
+      <c r="R22" s="29"/>
+      <c r="S22" s="27"/>
+      <c r="U22" s="29"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
@@ -3286,29 +3326,29 @@
         <v>203</v>
       </c>
     </row>
-    <row r="26" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
+    <row r="26" spans="1:21" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="26">
         <v>25</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="26">
         <v>25</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="11"/>
-      <c r="F26" s="16" t="s">
+      <c r="D26" s="27"/>
+      <c r="F26" s="28" t="s">
         <v>656</v>
       </c>
-      <c r="G26" s="11"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="11"/>
-      <c r="M26" s="11"/>
-      <c r="O26" s="12"/>
-      <c r="P26" s="11"/>
-      <c r="R26" s="12"/>
-      <c r="S26" s="11"/>
-      <c r="U26" s="12"/>
+      <c r="G26" s="27"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="27"/>
+      <c r="M26" s="27"/>
+      <c r="O26" s="29"/>
+      <c r="P26" s="27"/>
+      <c r="R26" s="29"/>
+      <c r="S26" s="27"/>
+      <c r="U26" s="29"/>
     </row>
     <row r="27" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">

</xml_diff>